<commit_message>
Updated wt3 test case.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_wt3.xlsx
+++ b/andes/cases/ieee14/ieee14_wt3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC41A634-63CB-5544-AC75-0A6F6077F5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C784CB2-6A52-7543-AAA0-5C30E8D3542B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="33600" windowHeight="16300" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="33600" windowHeight="16300" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="294">
   <si>
     <t>uid</t>
   </si>
@@ -2339,7 +2339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35E049C-6957-482F-A25F-1186A8D8FFB3}">
   <dimension ref="A1:BD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AM1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
     </sheetView>
@@ -2938,16 +2938,16 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2380FAD0-1118-4B99-8E7F-8DD4313D4F58}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2967,22 +2967,19 @@
         <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>257</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3002,18 +2999,15 @@
         <v>1000</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
         <v>1</v>
       </c>
     </row>

</xml_diff>